<commit_message>
reorder table by system
</commit_message>
<xml_diff>
--- a/manuscript/Table_S3.xlsx
+++ b/manuscript/Table_S3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/justine_hansen_mail_mcgill_ca/Documents/MisicLab/proj_receptors/manuscript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/justine_hansen_mail_mcgill_ca/Documents/MisicLab/proj_receptors/github/hansen_receptors/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{39DF3749-D078-43A5-AF17-B05BD19DFE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD1E3C1B-A098-43DA-B660-DFDCFA90CD60}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{39DF3749-D078-43A5-AF17-B05BD19DFE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E854AB17-2F57-42E3-9F9C-FB55563C6CB9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A9BF0D2D-F4F5-4604-A9C6-F8390957E683}"/>
   </bookViews>
@@ -543,7 +543,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -631,7 +631,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -955,29 +954,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D057157-771D-4F59-87A4-FD991BB3EEEB}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="76.28515625" customWidth="1"/>
-    <col min="14" max="14" width="38.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="76.33203125" customWidth="1"/>
+    <col min="14" max="14" width="38.33203125" customWidth="1"/>
     <col min="15" max="15" width="35" customWidth="1"/>
-    <col min="16" max="16" width="45.85546875" customWidth="1"/>
+    <col min="16" max="16" width="45.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1027,33 +1026,33 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2">
-        <v>28.4</v>
+        <v>33</v>
       </c>
       <c r="H2">
-        <v>8.8000000000000007</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
@@ -1062,45 +1061,42 @@
         <v>21</v>
       </c>
       <c r="L2">
-        <v>120</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>49</v>
+      </c>
+      <c r="E3">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>18</v>
-      </c>
       <c r="F3">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="G3">
-        <v>26.3</v>
+        <v>18.41</v>
       </c>
       <c r="H3">
-        <v>5.2</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
-        <v>20</v>
+      <c r="J3" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>
@@ -1108,367 +1104,348 @@
       <c r="L3">
         <v>90</v>
       </c>
-      <c r="M3" t="s">
-        <v>27</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>85</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
-        <v>36</v>
-      </c>
-      <c r="E4">
-        <v>24</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>27.8</v>
-      </c>
-      <c r="H4">
-        <v>6.9</v>
+      <c r="D4" s="3">
+        <v>37</v>
+      </c>
+      <c r="E4" s="3">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4">
+        <v>48.357300000000002</v>
+      </c>
+      <c r="H4" s="4">
+        <v>16.93366</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
       </c>
       <c r="L4">
-        <v>90</v>
-      </c>
-      <c r="M4" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="180">
+        <v>88</v>
+      </c>
+      <c r="O4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>65</v>
-      </c>
-      <c r="E5">
-        <v>49</v>
-      </c>
-      <c r="F5">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>33.729999999999997</v>
-      </c>
-      <c r="H5">
-        <v>9.73</v>
+        <v>40</v>
+      </c>
+      <c r="D5" s="3">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3">
+        <v>29</v>
+      </c>
+      <c r="G5" s="4">
+        <v>32.445639999999997</v>
+      </c>
+      <c r="H5" s="4">
+        <v>9.6861999999999995</v>
       </c>
       <c r="I5" t="s">
         <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="K5" t="s">
         <v>21</v>
       </c>
       <c r="L5">
-        <v>120</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>35</v>
+        <v>90</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>28.7</v>
+        <v>24</v>
       </c>
       <c r="H6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I6" t="s">
         <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
       </c>
       <c r="L6">
-        <v>120</v>
-      </c>
-      <c r="M6" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D7">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>28.2</v>
+        <v>31.06</v>
       </c>
       <c r="H7">
-        <v>5.7</v>
+        <v>7.7</v>
       </c>
       <c r="I7" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="8"/>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
       <c r="K7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" t="s">
-        <v>41</v>
+        <v>97</v>
+      </c>
+      <c r="L7">
+        <v>90</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>99</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="D8">
-        <v>29</v>
+        <v>174</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="G8">
-        <v>22.6</v>
+        <v>61</v>
       </c>
       <c r="H8">
-        <v>2.7</v>
+        <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="K8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="M8" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="3">
-        <v>3</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>41.14</v>
-      </c>
-      <c r="H9" s="4">
-        <v>9.9439829999999994</v>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>33.299999999999997</v>
       </c>
       <c r="I9" t="s">
         <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="L9">
         <v>120</v>
       </c>
-      <c r="M9" t="s">
-        <v>47</v>
-      </c>
       <c r="N9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="E10">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F10">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G10">
-        <v>25.9</v>
+        <v>33.4</v>
       </c>
       <c r="H10">
-        <v>5.3</v>
+        <v>9.17</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J10" t="s">
         <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="L10">
         <v>120</v>
       </c>
       <c r="M10" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15">
+        <v>142</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G11">
-        <v>36.6</v>
+        <v>28.4</v>
       </c>
       <c r="H11">
-        <v>9.0399999999999991</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="K11" t="s">
         <v>21</v>
@@ -1477,42 +1454,36 @@
         <v>120</v>
       </c>
       <c r="M11" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O11" t="s">
-        <v>57</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
       </c>
       <c r="D12">
+        <v>35</v>
+      </c>
+      <c r="E12">
         <v>18</v>
       </c>
-      <c r="E12">
-        <v>12</v>
-      </c>
       <c r="F12">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G12">
-        <v>30.5</v>
+        <v>26.3</v>
       </c>
       <c r="H12">
-        <v>9.5</v>
+        <v>5.2</v>
       </c>
       <c r="I12" t="s">
         <v>26</v>
@@ -1524,39 +1495,42 @@
         <v>21</v>
       </c>
       <c r="L12">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="M12" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="O12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="E13">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F13">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="G13">
-        <v>25.1</v>
+        <v>27.8</v>
       </c>
       <c r="H13">
-        <v>5.8</v>
+        <v>6.9</v>
       </c>
       <c r="I13" t="s">
         <v>19</v>
@@ -1571,183 +1545,177 @@
         <v>90</v>
       </c>
       <c r="M13" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3">
-        <v>30</v>
-      </c>
-      <c r="E14" s="3">
+      <c r="D14">
+        <v>65</v>
+      </c>
+      <c r="E14">
+        <v>49</v>
+      </c>
+      <c r="F14">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="H14">
+        <v>9.73</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="3">
-        <v>10</v>
-      </c>
-      <c r="G14" s="4">
-        <v>33.503</v>
-      </c>
-      <c r="H14" s="4">
-        <v>10.712809999999999</v>
-      </c>
-      <c r="I14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" t="s">
-        <v>65</v>
-      </c>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="L14">
         <v>120</v>
       </c>
       <c r="M14" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="O14" t="s">
-        <v>69</v>
+        <v>34</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>28.7</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15">
+        <v>120</v>
+      </c>
+      <c r="M15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>19</v>
+      </c>
+      <c r="E16">
         <v>11</v>
       </c>
-      <c r="F15">
-        <v>11</v>
-      </c>
-      <c r="G15">
-        <v>27.5</v>
-      </c>
-      <c r="H15">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="I15" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" t="s">
-        <v>72</v>
-      </c>
-      <c r="K15" t="s">
-        <v>66</v>
-      </c>
-      <c r="L15">
-        <v>60</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="105">
-      <c r="A16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>28.2</v>
+      </c>
+      <c r="H16">
+        <v>5.7</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D16">
-        <v>77</v>
-      </c>
-      <c r="E16">
-        <v>49</v>
-      </c>
-      <c r="F16">
-        <v>28</v>
-      </c>
-      <c r="G16">
-        <v>30.01</v>
-      </c>
-      <c r="H16">
-        <v>8.8699999999999992</v>
-      </c>
-      <c r="I16" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" t="s">
-        <v>54</v>
-      </c>
-      <c r="K16" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16">
-        <v>120</v>
-      </c>
-      <c r="M16" t="s">
-        <v>76</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O16" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" t="s">
-        <v>81</v>
-      </c>
       <c r="D17">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E17">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G17">
-        <v>33</v>
+        <v>22.6</v>
       </c>
       <c r="H17">
-        <v>13</v>
+        <v>2.7</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="J17" t="s">
         <v>20</v>
@@ -1756,86 +1724,95 @@
         <v>21</v>
       </c>
       <c r="L17">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18">
-        <v>49</v>
-      </c>
-      <c r="E18">
-        <v>16</v>
-      </c>
-      <c r="F18">
-        <v>33</v>
-      </c>
-      <c r="G18">
-        <v>18.41</v>
-      </c>
-      <c r="H18">
-        <v>0.56999999999999995</v>
+        <v>40</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>41.14</v>
+      </c>
+      <c r="H18" s="4">
+        <v>9.9439829999999994</v>
       </c>
       <c r="I18" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" t="s">
         <v>46</v>
       </c>
       <c r="K18" t="s">
         <v>21</v>
       </c>
       <c r="L18">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="M18" t="s">
+        <v>47</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>85</v>
+        <v>48</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="3">
-        <v>37</v>
-      </c>
-      <c r="E19" s="3">
-        <v>17</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="D19">
+        <v>59</v>
+      </c>
+      <c r="E19">
+        <v>41</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+      <c r="G19">
+        <v>25.9</v>
+      </c>
+      <c r="H19">
+        <v>5.3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
         <v>20</v>
-      </c>
-      <c r="G19" s="4">
-        <v>48.357300000000002</v>
-      </c>
-      <c r="H19" s="4">
-        <v>16.93366</v>
-      </c>
-      <c r="I19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" t="s">
-        <v>46</v>
       </c>
       <c r="K19" t="s">
         <v>21</v>
@@ -1843,422 +1820,425 @@
       <c r="L19">
         <v>120</v>
       </c>
+      <c r="M19" t="s">
+        <v>22</v>
+      </c>
       <c r="N19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="O19" t="s">
-        <v>89</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="120">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="3">
-        <v>55</v>
-      </c>
-      <c r="E20" s="3">
-        <v>26</v>
-      </c>
-      <c r="F20" s="3">
-        <v>29</v>
-      </c>
-      <c r="G20" s="4">
-        <v>32.445639999999997</v>
-      </c>
-      <c r="H20" s="4">
-        <v>9.6861999999999995</v>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>36.6</v>
+      </c>
+      <c r="H20">
+        <v>9.0399999999999991</v>
       </c>
       <c r="I20" t="s">
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="K20" t="s">
         <v>21</v>
       </c>
       <c r="L20">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="M20" t="s">
+        <v>55</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O20" s="10" t="s">
-        <v>91</v>
+        <v>56</v>
+      </c>
+      <c r="O20" t="s">
+        <v>57</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21">
         <v>18</v>
       </c>
-      <c r="D21">
-        <v>7</v>
-      </c>
       <c r="E21">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G21">
-        <v>24</v>
+        <v>30.5</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="I21" t="s">
         <v>26</v>
       </c>
       <c r="J21" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="K21" t="s">
         <v>21</v>
       </c>
       <c r="L21">
-        <v>80</v>
+        <v>120</v>
+      </c>
+      <c r="M21" t="s">
+        <v>60</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="G22">
-        <v>31.06</v>
+        <v>25.1</v>
       </c>
       <c r="H22">
-        <v>7.7</v>
+        <v>5.8</v>
       </c>
       <c r="I22" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="L22">
         <v>90</v>
       </c>
       <c r="M22" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="3">
+        <v>30</v>
+      </c>
+      <c r="E23" s="3">
+        <v>20</v>
+      </c>
+      <c r="F23" s="3">
+        <v>10</v>
+      </c>
+      <c r="G23" s="4">
+        <v>33.503</v>
+      </c>
+      <c r="H23" s="4">
+        <v>10.712809999999999</v>
+      </c>
+      <c r="I23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J23" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" t="s">
+        <v>66</v>
+      </c>
+      <c r="L23">
+        <v>120</v>
+      </c>
+      <c r="M23" t="s">
+        <v>67</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" t="s">
+        <v>69</v>
+      </c>
+      <c r="P23" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23">
-        <v>174</v>
-      </c>
-      <c r="E23">
-        <v>109</v>
-      </c>
-      <c r="F23">
-        <v>65</v>
-      </c>
-      <c r="G23">
-        <v>61</v>
-      </c>
-      <c r="H23">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="3">
+        <v>24</v>
+      </c>
+      <c r="E24" s="3">
+        <v>13</v>
+      </c>
+      <c r="F24" s="3">
         <v>11</v>
       </c>
-      <c r="I23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J23" t="s">
-        <v>66</v>
-      </c>
-      <c r="K23" t="s">
-        <v>103</v>
-      </c>
-      <c r="M23" t="s">
-        <v>104</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-      <c r="E24">
-        <v>6</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>43</v>
-      </c>
-      <c r="H24">
-        <v>4</v>
+      <c r="G24" s="4">
+        <v>40.445799999999998</v>
+      </c>
+      <c r="H24" s="4">
+        <v>11.712429999999999</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="J24" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="K24" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="L24">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="M24" t="s">
+        <v>122</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>123</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E25">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>26.6</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="H25">
-        <v>8</v>
+        <v>0.94</v>
       </c>
       <c r="I25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>111</v>
+        <v>102</v>
+      </c>
+      <c r="J25" t="s">
+        <v>66</v>
       </c>
       <c r="K25" t="s">
+        <v>146</v>
+      </c>
+      <c r="L25">
+        <v>30</v>
+      </c>
+      <c r="N25" t="s">
+        <v>147</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>37</v>
+      </c>
+      <c r="H26">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" t="s">
         <v>66</v>
       </c>
-      <c r="L25">
-        <v>90</v>
-      </c>
-      <c r="M25" t="s">
-        <v>112</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="K26" t="s">
+        <v>146</v>
+      </c>
+      <c r="L26" t="s">
+        <v>149</v>
+      </c>
+      <c r="N26" t="s">
+        <v>150</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>68.3</v>
+      </c>
+      <c r="H27">
+        <v>3.1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" t="s">
+        <v>66</v>
+      </c>
+      <c r="K27" t="s">
+        <v>146</v>
+      </c>
+      <c r="L27">
+        <v>180</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="3">
-        <v>8</v>
-      </c>
-      <c r="E26" s="3">
-        <v>7</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="4">
-        <v>31.688749999999999</v>
-      </c>
-      <c r="H26" s="4">
-        <v>8.9505549999999996</v>
-      </c>
-      <c r="I26" t="s">
-        <v>64</v>
-      </c>
-      <c r="J26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="D28">
+        <v>18</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>13</v>
+      </c>
+      <c r="G28">
+        <v>66.8</v>
+      </c>
+      <c r="H28">
+        <v>6.8</v>
+      </c>
+      <c r="I28" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28" t="s">
         <v>66</v>
       </c>
-      <c r="L26">
-        <v>120</v>
-      </c>
-      <c r="M26" t="s">
-        <v>116</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="3">
-        <v>24</v>
-      </c>
-      <c r="E27" s="3">
-        <v>13</v>
-      </c>
-      <c r="F27" s="3">
-        <v>11</v>
-      </c>
-      <c r="G27" s="4">
-        <v>40.445799999999998</v>
-      </c>
-      <c r="H27" s="4">
-        <v>11.712429999999999</v>
-      </c>
-      <c r="I27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J27" t="s">
-        <v>121</v>
-      </c>
-      <c r="K27" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27">
-        <v>120</v>
-      </c>
-      <c r="M27" t="s">
-        <v>122</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28">
-        <v>22</v>
-      </c>
-      <c r="E28">
-        <v>12</v>
-      </c>
-      <c r="F28">
-        <v>10</v>
-      </c>
-      <c r="G28">
-        <v>67.900000000000006</v>
-      </c>
-      <c r="H28">
-        <v>9.6</v>
-      </c>
-      <c r="I28" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="K28" t="s">
-        <v>126</v>
-      </c>
-      <c r="L28" s="8">
-        <v>60</v>
-      </c>
-      <c r="N28" t="s">
-        <v>127</v>
-      </c>
-      <c r="P28" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15">
+        <v>146</v>
+      </c>
+      <c r="L28">
+        <v>180</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -2269,24 +2249,24 @@
         <v>18</v>
       </c>
       <c r="D29">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E29">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F29">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G29">
-        <v>33.1</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="H29">
-        <v>11.2</v>
+        <v>9.6</v>
       </c>
       <c r="I29" t="s">
         <v>26</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" t="s">
         <v>46</v>
       </c>
       <c r="K29" t="s">
@@ -2295,14 +2275,14 @@
       <c r="L29">
         <v>60</v>
       </c>
-      <c r="N29" s="2" t="s">
-        <v>129</v>
+      <c r="N29" t="s">
+        <v>127</v>
       </c>
       <c r="P29" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>124</v>
       </c>
@@ -2313,24 +2293,24 @@
         <v>18</v>
       </c>
       <c r="D30">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E30">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F30">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G30">
-        <v>19.899999999999999</v>
+        <v>33.1</v>
       </c>
       <c r="H30">
-        <v>3.04</v>
+        <v>11.2</v>
       </c>
       <c r="I30" t="s">
         <v>26</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="J30" t="s">
         <v>46</v>
       </c>
       <c r="K30" t="s">
@@ -2340,36 +2320,36 @@
         <v>60</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
+        <v>129</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
       </c>
       <c r="D31">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="E31">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F31">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="G31">
-        <v>39.380000000000003</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="H31">
-        <v>5.05</v>
+        <v>3.04</v>
       </c>
       <c r="I31" t="s">
         <v>26</v>
@@ -2378,382 +2358,400 @@
         <v>46</v>
       </c>
       <c r="K31" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="L31">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="D32">
-        <v>204</v>
+        <v>6</v>
       </c>
       <c r="E32">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="F32">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>32.299999999999997</v>
+        <v>43</v>
       </c>
       <c r="H32">
-        <v>10.8</v>
+        <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="J32" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="K32" t="s">
-        <v>103</v>
-      </c>
-      <c r="L32" t="s">
-        <v>135</v>
-      </c>
-      <c r="M32" t="s">
-        <v>136</v>
+        <v>66</v>
+      </c>
+      <c r="L32">
+        <v>90</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>9</v>
       </c>
       <c r="G33">
-        <v>33.299999999999997</v>
+        <v>26.6</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
       </c>
       <c r="I33" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="J33" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="K33" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="L33">
-        <v>120</v>
+        <v>90</v>
+      </c>
+      <c r="M33" t="s">
+        <v>112</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="90">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
-      <c r="D34">
-        <v>77</v>
-      </c>
-      <c r="E34">
-        <v>50</v>
-      </c>
-      <c r="F34">
-        <v>27</v>
-      </c>
-      <c r="G34">
-        <v>33.4</v>
-      </c>
-      <c r="H34">
-        <v>9.17</v>
+      <c r="D34" s="3">
+        <v>8</v>
+      </c>
+      <c r="E34" s="3">
+        <v>7</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4">
+        <v>31.688749999999999</v>
+      </c>
+      <c r="H34" s="4">
+        <v>8.9505549999999996</v>
       </c>
       <c r="I34" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="J34" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="K34" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="L34">
         <v>120</v>
       </c>
       <c r="M34" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>143</v>
+        <v>117</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="P34" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="8">
-        <v>3</v>
-      </c>
-      <c r="E35" s="8">
-        <v>0</v>
-      </c>
-      <c r="F35" s="8">
-        <v>3</v>
-      </c>
-      <c r="G35" s="8">
-        <v>66.599999999999994</v>
-      </c>
-      <c r="H35" s="8">
-        <v>0.94</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J35" s="8" t="s">
+      <c r="D35">
+        <v>22</v>
+      </c>
+      <c r="E35">
+        <v>11</v>
+      </c>
+      <c r="F35">
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <v>27.5</v>
+      </c>
+      <c r="H35">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="I35" t="s">
+        <v>64</v>
+      </c>
+      <c r="J35" t="s">
+        <v>72</v>
+      </c>
+      <c r="K35" t="s">
         <v>66</v>
       </c>
-      <c r="K35" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="L35" s="8">
-        <v>30</v>
-      </c>
-      <c r="N35" t="s">
-        <v>147</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="L35">
+        <v>60</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G36">
-        <v>37</v>
+        <v>30.01</v>
       </c>
       <c r="H36">
-        <v>10.199999999999999</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="I36" t="s">
-        <v>102</v>
-      </c>
-      <c r="J36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J36" t="s">
+        <v>54</v>
+      </c>
+      <c r="K36" t="s">
         <v>66</v>
       </c>
-      <c r="K36" t="s">
-        <v>146</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="N36" t="s">
-        <v>150</v>
-      </c>
-      <c r="P36" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="L36">
+        <v>120</v>
+      </c>
+      <c r="M36" t="s">
+        <v>76</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O36" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C37" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G37">
-        <v>68.3</v>
+        <v>39.380000000000003</v>
       </c>
       <c r="H37">
-        <v>3.1</v>
+        <v>5.05</v>
       </c>
       <c r="I37" t="s">
-        <v>102</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>66</v>
+        <v>26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>46</v>
       </c>
       <c r="K37" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="L37">
-        <v>180</v>
+        <v>69</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D38">
-        <v>18</v>
+        <v>204</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="F38">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="G38">
-        <v>66.8</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="H38">
-        <v>6.8</v>
+        <v>10.8</v>
       </c>
       <c r="I38" t="s">
-        <v>102</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>66</v>
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>46</v>
       </c>
       <c r="K38" t="s">
-        <v>146</v>
-      </c>
-      <c r="L38">
-        <v>180</v>
+        <v>103</v>
+      </c>
+      <c r="L38" t="s">
+        <v>135</v>
+      </c>
+      <c r="M38" t="s">
+        <v>136</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{87E13921-6B3F-4777-8517-40296698F4EB}"/>
-    <hyperlink ref="N4" r:id="rId2" xr:uid="{79860EEF-20D4-424E-80FD-1DB1F6B1D332}"/>
-    <hyperlink ref="N8" r:id="rId3" xr:uid="{510D1C59-E467-4913-A6EB-129055C2A0DB}"/>
-    <hyperlink ref="N10" r:id="rId4" xr:uid="{05D3694E-C27D-4248-96FC-30DC0AA44B53}"/>
-    <hyperlink ref="N13" r:id="rId5" xr:uid="{EFCE4FE0-314F-4857-BB7A-8AE0EBF9C97D}"/>
-    <hyperlink ref="N6" r:id="rId6" xr:uid="{163E2F68-43B1-4C85-86EF-54482DB69F3D}"/>
-    <hyperlink ref="N12" r:id="rId7" xr:uid="{0C7990C3-146A-448D-B5D2-8E01BDF15391}"/>
-    <hyperlink ref="N3" r:id="rId8" xr:uid="{5953D8E2-1521-4018-8D1E-9BEB275C7D90}"/>
-    <hyperlink ref="N7" r:id="rId9" xr:uid="{CB647699-17AF-4C41-A7F0-779CCC56D7CD}"/>
-    <hyperlink ref="N5" r:id="rId10" display="gallezot2010" xr:uid="{804AA54E-8B47-4DB2-B95F-7DB8A14C7A7B}"/>
-    <hyperlink ref="O3" r:id="rId11" xr:uid="{D154E147-D1EB-4582-A4D6-BAD5336E3491}"/>
-    <hyperlink ref="O7" r:id="rId12" xr:uid="{65B808F4-FE24-4102-90DA-D5F9E27ED645}"/>
-    <hyperlink ref="N9" r:id="rId13" xr:uid="{96A1777C-4019-430B-9159-0B7EB0DF234C}"/>
-    <hyperlink ref="N11" r:id="rId14" xr:uid="{AED6C02C-CF4F-45B0-A23A-586F55A362A5}"/>
-    <hyperlink ref="N14" r:id="rId15" xr:uid="{E33ABFB7-0167-4385-83EA-F4786DCA6AF2}"/>
-    <hyperlink ref="N15" r:id="rId16" xr:uid="{11166F32-CEBD-4011-AFD6-CD24FCA3BF18}"/>
-    <hyperlink ref="N16" r:id="rId17" xr:uid="{BCB08B45-C756-4687-98F8-12F4506F6EC0}"/>
-    <hyperlink ref="N17" r:id="rId18" xr:uid="{5CEAF98C-8F73-4F96-AF36-2B61D6A35C6B}"/>
-    <hyperlink ref="N18" r:id="rId19" xr:uid="{1CE7E628-EABE-41B1-A280-001C0D1752C0}"/>
-    <hyperlink ref="N19" r:id="rId20" xr:uid="{59664589-391A-4753-A16D-660B11F300BE}"/>
-    <hyperlink ref="N20" r:id="rId21" xr:uid="{4F1EB123-6527-49C1-8330-0235AA32819B}"/>
-    <hyperlink ref="N21" r:id="rId22" xr:uid="{61D3AE50-A47F-41AF-B568-F11327D6D0F5}"/>
-    <hyperlink ref="N22" r:id="rId23" xr:uid="{7B5C9C40-B72B-4CAD-9DAE-558E81676413}"/>
-    <hyperlink ref="N23" r:id="rId24" xr:uid="{6A220D4C-EA1D-45B9-A121-1AF5D5C069DF}"/>
-    <hyperlink ref="N24" r:id="rId25" xr:uid="{772C6CAD-B6D6-47A6-A457-32D333D8D05D}"/>
-    <hyperlink ref="O24" r:id="rId26" xr:uid="{C0935F29-4E32-4C59-A741-72D6C9412CBA}"/>
-    <hyperlink ref="N25" r:id="rId27" xr:uid="{D479FC74-1851-48B2-8606-342B561BF8BE}"/>
-    <hyperlink ref="N26" r:id="rId28" display="gallezot2017" xr:uid="{C8530177-1A02-4B31-9D92-CC010B80D19C}"/>
-    <hyperlink ref="O26" r:id="rId29" xr:uid="{6DB61459-CAC6-4198-AE8C-54FF48C54F06}"/>
-    <hyperlink ref="N27" r:id="rId30" xr:uid="{6DB0DC8C-2796-441F-9C58-AC615F6E385A}"/>
-    <hyperlink ref="N29" r:id="rId31" xr:uid="{AD512145-4DC3-424A-8829-2CE2D63F974B}"/>
-    <hyperlink ref="N30" r:id="rId32" xr:uid="{F076B56E-70C7-4251-A14B-D6D01B4EE724}"/>
-    <hyperlink ref="N31" r:id="rId33" xr:uid="{2C5AAFA5-8766-4367-BA12-618AB320DD66}"/>
-    <hyperlink ref="N32" r:id="rId34" xr:uid="{9B445026-E7E3-40A7-8A80-B4A224AC5FF9}"/>
-    <hyperlink ref="N33" r:id="rId35" xr:uid="{9030A647-A56B-4A37-8261-79375DE31022}"/>
-    <hyperlink ref="N34" r:id="rId36" xr:uid="{5A4951AC-672B-4E35-BD01-9278074C37A6}"/>
-    <hyperlink ref="N37" r:id="rId37" xr:uid="{68D3E693-A5B8-4AA3-9DA4-A46D8327F50F}"/>
-    <hyperlink ref="N38" r:id="rId38" xr:uid="{23F98EC5-97D4-40C9-81FC-4EABC809B611}"/>
-    <hyperlink ref="P5" r:id="rId39" xr:uid="{3A928C38-6F2F-43A7-9E4A-B75F8B0A31C0}"/>
-    <hyperlink ref="P9" r:id="rId40" xr:uid="{83F065D9-A724-4DA2-8EE8-D0EC91236222}"/>
-    <hyperlink ref="P11" r:id="rId41" xr:uid="{7D097A03-44B1-4358-8523-FB801A0F69F9}"/>
-    <hyperlink ref="P14" r:id="rId42" xr:uid="{841F2567-B4B2-45F7-9866-3F831FC4F917}"/>
-    <hyperlink ref="P16" r:id="rId43" xr:uid="{931FE503-3A19-49CF-9394-A6543F088054}"/>
-    <hyperlink ref="P19" r:id="rId44" xr:uid="{87ECE724-0A01-4DA1-9B56-2D48EFAEF9B9}"/>
-    <hyperlink ref="P20" r:id="rId45" xr:uid="{B14B7728-34EF-4E7C-B43E-B57FFC194E4F}"/>
-    <hyperlink ref="P22" r:id="rId46" xr:uid="{69211328-FF57-4849-8EAC-49CD2C1CA95B}"/>
-    <hyperlink ref="P26" r:id="rId47" xr:uid="{13898C16-FF95-465A-A621-AE33789FD85C}"/>
-    <hyperlink ref="P27" r:id="rId48" xr:uid="{0CFD580D-3D17-42DF-B88A-2373C76E1799}"/>
-    <hyperlink ref="P15" r:id="rId49" xr:uid="{612529EC-B549-4775-83A0-8166D5A7A58A}"/>
-    <hyperlink ref="P31" r:id="rId50" xr:uid="{B65C8C33-E608-4ED2-915F-50C6731492AB}"/>
-    <hyperlink ref="P18" r:id="rId51" xr:uid="{B30F51C2-26D2-408E-9767-3C46A2F51448}"/>
-    <hyperlink ref="P30" r:id="rId52" xr:uid="{E9EA41C8-B36E-4ACE-822B-E8EE297A5CBE}"/>
-    <hyperlink ref="P34" r:id="rId53" xr:uid="{C472DC1F-E604-42F1-9F65-AB1FDB45806D}"/>
-    <hyperlink ref="P28" r:id="rId54" xr:uid="{6A98BDF8-F46E-4CEF-A21A-1C30599B1603}"/>
-    <hyperlink ref="P29" r:id="rId55" xr:uid="{A34B4783-63E7-4A74-99E2-416EC946E360}"/>
-    <hyperlink ref="P35" r:id="rId56" xr:uid="{8D73B688-E34C-4F49-B1A2-A6916A53DA1C}"/>
-    <hyperlink ref="P36" r:id="rId57" xr:uid="{048AFB6B-2BAB-43B7-B89F-4E670211C542}"/>
-    <hyperlink ref="P37" r:id="rId58" xr:uid="{279D0D45-D8E3-4BB4-A616-C42E08639772}"/>
-    <hyperlink ref="P38" r:id="rId59" xr:uid="{6DA0560C-0652-45FA-A012-758550EEA74B}"/>
-    <hyperlink ref="O9" r:id="rId60" xr:uid="{D69BCCFF-4DD5-47DA-9391-A6CA78C521E4}"/>
+    <hyperlink ref="N11" r:id="rId1" xr:uid="{87E13921-6B3F-4777-8517-40296698F4EB}"/>
+    <hyperlink ref="N13" r:id="rId2" xr:uid="{79860EEF-20D4-424E-80FD-1DB1F6B1D332}"/>
+    <hyperlink ref="N17" r:id="rId3" xr:uid="{510D1C59-E467-4913-A6EB-129055C2A0DB}"/>
+    <hyperlink ref="N19" r:id="rId4" xr:uid="{05D3694E-C27D-4248-96FC-30DC0AA44B53}"/>
+    <hyperlink ref="N22" r:id="rId5" xr:uid="{EFCE4FE0-314F-4857-BB7A-8AE0EBF9C97D}"/>
+    <hyperlink ref="N15" r:id="rId6" xr:uid="{163E2F68-43B1-4C85-86EF-54482DB69F3D}"/>
+    <hyperlink ref="N21" r:id="rId7" xr:uid="{0C7990C3-146A-448D-B5D2-8E01BDF15391}"/>
+    <hyperlink ref="N12" r:id="rId8" xr:uid="{5953D8E2-1521-4018-8D1E-9BEB275C7D90}"/>
+    <hyperlink ref="N16" r:id="rId9" xr:uid="{CB647699-17AF-4C41-A7F0-779CCC56D7CD}"/>
+    <hyperlink ref="N14" r:id="rId10" display="gallezot2010" xr:uid="{804AA54E-8B47-4DB2-B95F-7DB8A14C7A7B}"/>
+    <hyperlink ref="O12" r:id="rId11" xr:uid="{D154E147-D1EB-4582-A4D6-BAD5336E3491}"/>
+    <hyperlink ref="O16" r:id="rId12" xr:uid="{65B808F4-FE24-4102-90DA-D5F9E27ED645}"/>
+    <hyperlink ref="N18" r:id="rId13" xr:uid="{96A1777C-4019-430B-9159-0B7EB0DF234C}"/>
+    <hyperlink ref="N20" r:id="rId14" xr:uid="{AED6C02C-CF4F-45B0-A23A-586F55A362A5}"/>
+    <hyperlink ref="N23" r:id="rId15" xr:uid="{E33ABFB7-0167-4385-83EA-F4786DCA6AF2}"/>
+    <hyperlink ref="N35" r:id="rId16" xr:uid="{11166F32-CEBD-4011-AFD6-CD24FCA3BF18}"/>
+    <hyperlink ref="N36" r:id="rId17" xr:uid="{BCB08B45-C756-4687-98F8-12F4506F6EC0}"/>
+    <hyperlink ref="N2" r:id="rId18" xr:uid="{5CEAF98C-8F73-4F96-AF36-2B61D6A35C6B}"/>
+    <hyperlink ref="N3" r:id="rId19" xr:uid="{1CE7E628-EABE-41B1-A280-001C0D1752C0}"/>
+    <hyperlink ref="N4" r:id="rId20" xr:uid="{59664589-391A-4753-A16D-660B11F300BE}"/>
+    <hyperlink ref="N5" r:id="rId21" xr:uid="{4F1EB123-6527-49C1-8330-0235AA32819B}"/>
+    <hyperlink ref="N6" r:id="rId22" xr:uid="{61D3AE50-A47F-41AF-B568-F11327D6D0F5}"/>
+    <hyperlink ref="N7" r:id="rId23" xr:uid="{7B5C9C40-B72B-4CAD-9DAE-558E81676413}"/>
+    <hyperlink ref="N8" r:id="rId24" xr:uid="{6A220D4C-EA1D-45B9-A121-1AF5D5C069DF}"/>
+    <hyperlink ref="N32" r:id="rId25" xr:uid="{772C6CAD-B6D6-47A6-A457-32D333D8D05D}"/>
+    <hyperlink ref="O32" r:id="rId26" xr:uid="{C0935F29-4E32-4C59-A741-72D6C9412CBA}"/>
+    <hyperlink ref="N33" r:id="rId27" xr:uid="{D479FC74-1851-48B2-8606-342B561BF8BE}"/>
+    <hyperlink ref="N34" r:id="rId28" display="gallezot2017" xr:uid="{C8530177-1A02-4B31-9D92-CC010B80D19C}"/>
+    <hyperlink ref="O34" r:id="rId29" xr:uid="{6DB61459-CAC6-4198-AE8C-54FF48C54F06}"/>
+    <hyperlink ref="N24" r:id="rId30" xr:uid="{6DB0DC8C-2796-441F-9C58-AC615F6E385A}"/>
+    <hyperlink ref="N30" r:id="rId31" xr:uid="{AD512145-4DC3-424A-8829-2CE2D63F974B}"/>
+    <hyperlink ref="N31" r:id="rId32" xr:uid="{F076B56E-70C7-4251-A14B-D6D01B4EE724}"/>
+    <hyperlink ref="N37" r:id="rId33" xr:uid="{2C5AAFA5-8766-4367-BA12-618AB320DD66}"/>
+    <hyperlink ref="N38" r:id="rId34" xr:uid="{9B445026-E7E3-40A7-8A80-B4A224AC5FF9}"/>
+    <hyperlink ref="N9" r:id="rId35" xr:uid="{9030A647-A56B-4A37-8261-79375DE31022}"/>
+    <hyperlink ref="N10" r:id="rId36" xr:uid="{5A4951AC-672B-4E35-BD01-9278074C37A6}"/>
+    <hyperlink ref="N27" r:id="rId37" xr:uid="{68D3E693-A5B8-4AA3-9DA4-A46D8327F50F}"/>
+    <hyperlink ref="N28" r:id="rId38" xr:uid="{23F98EC5-97D4-40C9-81FC-4EABC809B611}"/>
+    <hyperlink ref="P14" r:id="rId39" xr:uid="{3A928C38-6F2F-43A7-9E4A-B75F8B0A31C0}"/>
+    <hyperlink ref="P18" r:id="rId40" xr:uid="{83F065D9-A724-4DA2-8EE8-D0EC91236222}"/>
+    <hyperlink ref="P20" r:id="rId41" xr:uid="{7D097A03-44B1-4358-8523-FB801A0F69F9}"/>
+    <hyperlink ref="P23" r:id="rId42" xr:uid="{841F2567-B4B2-45F7-9866-3F831FC4F917}"/>
+    <hyperlink ref="P36" r:id="rId43" xr:uid="{931FE503-3A19-49CF-9394-A6543F088054}"/>
+    <hyperlink ref="P4" r:id="rId44" xr:uid="{87ECE724-0A01-4DA1-9B56-2D48EFAEF9B9}"/>
+    <hyperlink ref="P5" r:id="rId45" xr:uid="{B14B7728-34EF-4E7C-B43E-B57FFC194E4F}"/>
+    <hyperlink ref="P7" r:id="rId46" xr:uid="{69211328-FF57-4849-8EAC-49CD2C1CA95B}"/>
+    <hyperlink ref="P34" r:id="rId47" xr:uid="{13898C16-FF95-465A-A621-AE33789FD85C}"/>
+    <hyperlink ref="P24" r:id="rId48" xr:uid="{0CFD580D-3D17-42DF-B88A-2373C76E1799}"/>
+    <hyperlink ref="P35" r:id="rId49" xr:uid="{612529EC-B549-4775-83A0-8166D5A7A58A}"/>
+    <hyperlink ref="P37" r:id="rId50" xr:uid="{B65C8C33-E608-4ED2-915F-50C6731492AB}"/>
+    <hyperlink ref="P3" r:id="rId51" xr:uid="{B30F51C2-26D2-408E-9767-3C46A2F51448}"/>
+    <hyperlink ref="P31" r:id="rId52" xr:uid="{E9EA41C8-B36E-4ACE-822B-E8EE297A5CBE}"/>
+    <hyperlink ref="P10" r:id="rId53" xr:uid="{C472DC1F-E604-42F1-9F65-AB1FDB45806D}"/>
+    <hyperlink ref="P29" r:id="rId54" xr:uid="{6A98BDF8-F46E-4CEF-A21A-1C30599B1603}"/>
+    <hyperlink ref="P30" r:id="rId55" xr:uid="{A34B4783-63E7-4A74-99E2-416EC946E360}"/>
+    <hyperlink ref="P25" r:id="rId56" xr:uid="{8D73B688-E34C-4F49-B1A2-A6916A53DA1C}"/>
+    <hyperlink ref="P26" r:id="rId57" xr:uid="{048AFB6B-2BAB-43B7-B89F-4E670211C542}"/>
+    <hyperlink ref="P27" r:id="rId58" xr:uid="{279D0D45-D8E3-4BB4-A616-C42E08639772}"/>
+    <hyperlink ref="P28" r:id="rId59" xr:uid="{6DA0560C-0652-45FA-A012-758550EEA74B}"/>
+    <hyperlink ref="O18" r:id="rId60" xr:uid="{D69BCCFF-4DD5-47DA-9391-A6CA78C521E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId61"/>

</xml_diff>

<commit_message>
add NMDA + bug fix in make_receptor_matrix
</commit_message>
<xml_diff>
--- a/manuscript/Table_S3.xlsx
+++ b/manuscript/Table_S3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/justine_hansen_mail_mcgill_ca/Documents/MisicLab/proj_receptors/github/hansen_receptors/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{39DF3749-D078-43A5-AF17-B05BD19DFE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E854AB17-2F57-42E3-9F9C-FB55563C6CB9}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{39DF3749-D078-43A5-AF17-B05BD19DFE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8037567-EC3A-45F0-9F96-A948413D1196}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A9BF0D2D-F4F5-4604-A9C6-F8390957E683}"/>
   </bookViews>
@@ -954,13 +954,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D057157-771D-4F59-87A4-FD991BB3EEEB}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
     <col min="4" max="4" width="5.88671875" customWidth="1"/>
     <col min="5" max="5" width="7.88671875" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" customWidth="1"/>

</xml_diff>